<commit_message>
Updated test fixtures for secret pdfs
</commit_message>
<xml_diff>
--- a/tests/fixtures/secret_pdf_scanned.xlsx
+++ b/tests/fixtures/secret_pdf_scanned.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/xnat-uploader/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E4AB64-0FDB-6640-8D9C-576D35071135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E927824-C6AA-504A-89B4-4B949FEF07CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40160" yWindow="2780" windowWidth="29340" windowHeight="15200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -174,7 +174,7 @@
     <t>DICOM:SeriesNumber</t>
   </si>
   <si>
-    <t>10001_CT1</t>
+    <t>10001_CT1_6168</t>
   </si>
 </sst>
 </file>
@@ -643,7 +643,7 @@
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>